<commit_message>
random forest regressor feature clustering
</commit_message>
<xml_diff>
--- a/data/metadata/Huishi charts OGTT vs insulin and RBG week 8 predictors.xlsx
+++ b/data/metadata/Huishi charts OGTT vs insulin and RBG week 8 predictors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nile_rat_multiomics\data\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A4D3262-39D6-47A8-BBD4-6FC93A7103C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E4DEF3-176F-4EB8-9504-3C2E7A77D52D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10110" yWindow="5640" windowWidth="24800" windowHeight="12570" xr2:uid="{4D867CAF-6E99-884A-974B-94137FA2F999}"/>
+    <workbookView minimized="1" xWindow="-26790" yWindow="16035" windowWidth="18885" windowHeight="8445" xr2:uid="{4D867CAF-6E99-884A-974B-94137FA2F999}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -10500,7 +10500,7 @@
   <dimension ref="A1:V69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H72" sqref="H72"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>

</xml_diff>